<commit_message>
Implementa a correção do endereço das mensagens recebidas através do whatsapp.
</commit_message>
<xml_diff>
--- a/data/gastos.xlsx
+++ b/data/gastos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45956.56062929736</v>
+        <v>45956.56062929398</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -474,6 +474,24 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>uber</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45957.86045812783</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>gasto</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>mercado</t>
         </is>
       </c>
     </row>

</xml_diff>